<commit_message>
Added Excel and test cases for heart attack Predictor
</commit_message>
<xml_diff>
--- a/Heartihealth/src/main/resources/TestData/TestData.xlsx
+++ b/Heartihealth/src/main/resources/TestData/TestData.xlsx
@@ -3,41 +3,63 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lavanya.jami\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{943D8EC0-CF4D-4276-B3B6-C1FDF2EE8D67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{ACE53D83-90A6-409F-B488-1EFC6C7E9266}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{248BB9E6-8075-4E41-ABA8-A549F6C61C4D}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="20670" windowHeight="11700" firstSheet="1" activeTab="1" xr2:uid="{248BB9E6-8075-4E41-ABA8-A549F6C61C4D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginWithValiddata" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginWithInvalidData" sheetId="2" r:id="rId2"/>
+    <sheet name="HeartAttackCalculator" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:I2"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>testuser@example.com</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -60,13 +82,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -379,12 +405,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0798BC6-FEEF-4039-8C26-EB37D530F25D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1">
+        <v>12345</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89D0FE6A-9D63-4457-AB8D-EFB0DD019DF5}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>123456</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{096AB96F-B871-4C8B-9B0D-A6C02B1EBD5A}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{812B4E43-E0BB-4D01-ADFD-D0220FEACE98}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36EC8158-EB5E-43A4-B119-A10409305ADF}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>